<commit_message>
Revert "Merge branch 'master' into i1076-NN-Recurrent-Conv"
This reverts commit c5609343ab1639024141d48d4cea94e25880d600, reversing
changes made to 64d8415741d93e3672c3b71a97dd2a4ceb17addf.
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/construction_properties.xlsx
+++ b/cea/databases/CH/archetypes/construction_properties.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\GitHub\CEAforArcGIS\cea\databases\CH\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\GitHub\CityEnergyAnalyst\cea\databases\CH\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18135" yWindow="465" windowWidth="21255" windowHeight="22020" tabRatio="785" activeTab="3"/>
+    <workbookView xWindow="18135" yWindow="465" windowWidth="21255" windowHeight="22020" tabRatio="785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5753" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5751" uniqueCount="78">
   <si>
     <t>Code</t>
   </si>
@@ -265,12 +265,6 @@
   </si>
   <si>
     <t>type_el</t>
-  </si>
-  <si>
-    <t>rhum_min_pc</t>
-  </si>
-  <si>
-    <t>rhum_max_pc</t>
   </si>
 </sst>
 </file>
@@ -12148,7 +12142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M217"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -17051,7 +17045,7 @@
         <v>T1</v>
       </c>
       <c r="F188" s="3" t="str">
-        <f t="shared" ref="F188:F193" si="2">F92</f>
+        <f>F92</f>
         <v>T1</v>
       </c>
       <c r="G188" s="3" t="str">
@@ -17080,7 +17074,7 @@
         <v>T1</v>
       </c>
       <c r="F189" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>F93</f>
         <v>T1</v>
       </c>
       <c r="G189" s="3" t="str">
@@ -17109,7 +17103,7 @@
         <v>T1</v>
       </c>
       <c r="F190" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>F94</f>
         <v>T1</v>
       </c>
       <c r="G190" s="3" t="str">
@@ -17138,7 +17132,7 @@
         <v>T1</v>
       </c>
       <c r="F191" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>F95</f>
         <v>T1</v>
       </c>
       <c r="G191" s="3" t="str">
@@ -17167,7 +17161,7 @@
         <v>T3</v>
       </c>
       <c r="F192" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>F96</f>
         <v>T3</v>
       </c>
       <c r="G192" s="3" t="str">
@@ -17196,7 +17190,7 @@
         <v>T3</v>
       </c>
       <c r="F193" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>F97</f>
         <v>T3</v>
       </c>
       <c r="G193" s="3" t="str">
@@ -24245,10 +24239,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24262,7 +24256,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -24281,14 +24275,8 @@
       <c r="F1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
@@ -24307,14 +24295,8 @@
       <c r="F2" s="6">
         <v>10</v>
       </c>
-      <c r="G2" s="6">
-        <v>30</v>
-      </c>
-      <c r="H2" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -24333,14 +24315,8 @@
       <c r="F3" s="6">
         <v>10</v>
       </c>
-      <c r="G3" s="6">
-        <v>30</v>
-      </c>
-      <c r="H3" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>24</v>
       </c>
@@ -24356,17 +24332,11 @@
       <c r="E4" s="5">
         <v>21</v>
       </c>
-      <c r="F4" s="6">
-        <v>10</v>
-      </c>
-      <c r="G4" s="6">
-        <v>30</v>
-      </c>
-      <c r="H4" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
@@ -24382,17 +24352,11 @@
       <c r="E5" s="5">
         <v>12</v>
       </c>
-      <c r="F5" s="6">
-        <v>10</v>
-      </c>
-      <c r="G5" s="6">
-        <v>30</v>
-      </c>
-      <c r="H5" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>26</v>
       </c>
@@ -24408,17 +24372,11 @@
       <c r="E6" s="5">
         <v>12</v>
       </c>
-      <c r="F6" s="6">
-        <v>8</v>
-      </c>
-      <c r="G6" s="6">
-        <v>30</v>
-      </c>
-      <c r="H6" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
@@ -24434,17 +24392,11 @@
       <c r="E7" s="5">
         <v>12</v>
       </c>
-      <c r="F7" s="6">
-        <v>10</v>
-      </c>
-      <c r="G7" s="6">
-        <v>30</v>
-      </c>
-      <c r="H7" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>27</v>
       </c>
@@ -24460,18 +24412,12 @@
       <c r="E8" s="5">
         <v>12</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="9">
         <f t="shared" ref="F8" si="0">111*0.15+10*0.85</f>
         <v>25.15</v>
       </c>
-      <c r="G8" s="6">
-        <v>30</v>
-      </c>
-      <c r="H8" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
@@ -24487,17 +24433,11 @@
       <c r="E9" s="5">
         <v>12</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="9">
         <v>31</v>
       </c>
-      <c r="G9" s="6">
-        <v>30</v>
-      </c>
-      <c r="H9" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>29</v>
       </c>
@@ -24513,17 +24453,11 @@
       <c r="E10" s="5">
         <v>12</v>
       </c>
-      <c r="F10" s="6">
-        <v>8</v>
-      </c>
-      <c r="G10" s="6">
-        <v>30</v>
-      </c>
-      <c r="H10" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>30</v>
       </c>
@@ -24539,17 +24473,11 @@
       <c r="E11" s="5">
         <v>21</v>
       </c>
-      <c r="F11" s="6">
-        <v>10</v>
-      </c>
-      <c r="G11" s="6">
-        <v>30</v>
-      </c>
-      <c r="H11" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>31</v>
       </c>
@@ -24565,17 +24493,11 @@
       <c r="E12" s="5">
         <v>12</v>
       </c>
-      <c r="F12" s="6">
-        <v>10</v>
-      </c>
-      <c r="G12" s="6">
-        <v>30</v>
-      </c>
-      <c r="H12" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
@@ -24591,17 +24513,11 @@
       <c r="E13" s="5">
         <v>12</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="9">
         <v>36</v>
       </c>
-      <c r="G13" s="6">
-        <v>30</v>
-      </c>
-      <c r="H13" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>33</v>
       </c>
@@ -24617,17 +24533,11 @@
       <c r="E14" s="5">
         <v>12</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="9">
         <v>36</v>
       </c>
-      <c r="G14" s="6">
-        <v>30</v>
-      </c>
-      <c r="H14" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
@@ -24643,17 +24553,11 @@
       <c r="E15" s="5">
         <v>12</v>
       </c>
-      <c r="F15" s="6">
-        <v>0</v>
-      </c>
-      <c r="G15" s="6">
-        <v>30</v>
-      </c>
-      <c r="H15" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>35</v>
       </c>
@@ -24669,17 +24573,11 @@
       <c r="E16" s="5">
         <v>-5</v>
       </c>
-      <c r="F16" s="6">
-        <v>0</v>
-      </c>
-      <c r="G16" s="6">
-        <v>30</v>
-      </c>
-      <c r="H16" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>46</v>
       </c>
@@ -24695,18 +24593,12 @@
       <c r="E17" s="5">
         <v>12</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="9">
         <f>F9</f>
         <v>31</v>
       </c>
-      <c r="G17" s="6">
-        <v>30</v>
-      </c>
-      <c r="H17" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>47</v>
       </c>
@@ -24722,17 +24614,11 @@
       <c r="E18" s="5">
         <v>12</v>
       </c>
-      <c r="F18" s="6">
-        <v>10</v>
-      </c>
-      <c r="G18" s="6">
-        <v>30</v>
-      </c>
-      <c r="H18" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F18" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>48</v>
       </c>
@@ -24748,14 +24634,8 @@
       <c r="E19" s="5">
         <v>12</v>
       </c>
-      <c r="F19" s="6">
-        <v>10</v>
-      </c>
-      <c r="G19" s="6">
-        <v>30</v>
-      </c>
-      <c r="H19" s="6">
-        <v>70</v>
+      <c r="F19" s="9">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>